<commit_message>
The dcf template is now working
</commit_message>
<xml_diff>
--- a/resources/comparables_analysis.xlsx
+++ b/resources/comparables_analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lawrencelim/Projects/python-projects/pyfinny/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9601767-FF75-8642-8D1B-F0622643C49C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79EA1B79-2C0A-974B-84D4-EE0499ACE860}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="700" windowWidth="27040" windowHeight="16860" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8840" yWindow="21600" windowWidth="21600" windowHeight="16200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_CIQHiddenCacheSheet" sheetId="1" state="veryHidden" r:id="rId1"/>
@@ -818,7 +818,7 @@
   <dimension ref="A1:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -835,8 +835,8 @@
     <col min="11" max="11" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="26" width="9.1640625" style="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.1640625" style="1"/>
+    <col min="14" max="30" width="9.1640625" style="1" customWidth="1"/>
+    <col min="31" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>